<commit_message>
xleash, test: enhance recursive real excel.
+ Improve ABCSheet docs.
</commit_message>
<xml_diff>
--- a/tests/recursive.xlsx
+++ b/tests/recursive.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>#B1(D):..(DR):[“pipe”, [“odict”, “recurse”]]</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>#BAD1:"filter"</t>
+  </si>
+  <si>
+    <t>No Recurse</t>
   </si>
 </sst>
 </file>
@@ -438,28 +441,28 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6328125"/>
-    <col min="2" max="2" width="31.1796875"/>
-    <col min="3" max="3" width="37.453125"/>
-    <col min="4" max="1025" width="11.54296875"/>
+    <col min="1" max="1" width="27.5703125"/>
+    <col min="2" max="2" width="31.140625"/>
+    <col min="3" max="3" width="37.42578125"/>
+    <col min="4" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -467,7 +470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -475,7 +478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -483,12 +486,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -496,7 +507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -507,7 +518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -518,7 +529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -547,14 +558,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.54296875"/>
-    <col min="2" max="2" width="20.90625"/>
-    <col min="3" max="1025" width="11.54296875"/>
+    <col min="1" max="1" width="11.5703125"/>
+    <col min="2" max="2" width="20.85546875"/>
+    <col min="3" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>11</v>
       </c>
@@ -568,7 +579,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>21</v>
       </c>
@@ -582,7 +593,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D5" s="1"/>
       <c r="E5">
         <v>65</v>
@@ -591,16 +602,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -608,7 +619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -616,7 +627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -635,22 +646,22 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="11.54296875"/>
+    <col min="1" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D4">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F7">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
xlasso: Imporve recursive-context reporting.
+ tests: Compare stripped-strings.
</commit_message>
<xml_diff>
--- a/tests/recursive.xlsx
+++ b/tests/recursive.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>#B1(D):..(DR):[“pipe”, [“odict”, “recurse”]]</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>No Recurse</t>
+  </si>
+  <si>
+    <t>Empty</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -495,48 +498,53 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>31</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
xleash: AMIDST impl p-eval filter.
+ Recursive-filter accepts sub-filters.
+ real_excel: Extend checks (empty, eval)
+ FIX forgotten DTs on _capture!
  + FIX minor bad err-msg in parse_call_spec().
+ Separate pipe-filter from Ranger.
</commit_message>
<xml_diff>
--- a/tests/recursive.xlsx
+++ b/tests/recursive.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="211"/>
+    <workbookView xWindow="2265" yWindow="1335" windowWidth="16380" windowHeight="8190" tabRatio="358"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="1" r:id="rId1"/>
     <sheet name="3" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="3" r:id="rId3"/>
+    <sheet name="eval sheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>#B1(D):..(DR):[“pipe”, [“odict”, “recurse”]]</t>
   </si>
@@ -91,6 +92,36 @@
   </si>
   <si>
     <t>Empty</t>
+  </si>
+  <si>
+    <t>P-eval</t>
+  </si>
+  <si>
+    <t>dict(a_dict=1)</t>
+  </si>
+  <si>
+    <t>EVAL_COL</t>
+  </si>
+  <si>
+    <t>NO_EVAL</t>
+  </si>
+  <si>
+    <t>a'+4</t>
+  </si>
+  <si>
+    <t>bad boy</t>
+  </si>
+  <si>
+    <t>a=1; a+5</t>
+  </si>
+  <si>
+    <t>[1,2,3]</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>#eval sheet!::{"opts": {"lax": true}, "func": "pipe", "args":[["df", {"index_col": null}]]}</t>
   </si>
 </sst>
 </file>
@@ -136,10 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -502,49 +534,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>31</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -682,4 +722,60 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
xleash: Impl PY filter!
</commit_message>
<xml_diff>
--- a/tests/recursive.xlsx
+++ b/tests/recursive.xlsx
@@ -121,7 +121,7 @@
     <t>bus</t>
   </si>
   <si>
-    <t>#eval sheet!::{"opts": {"lax": true}, "func": "pipe", "args":[["df", {"index_col": null}], ["pyeval", ["numpy"]]]}</t>
+    <t>#eval sheet!::{"opts": {"lax": true}, "func": "pipe", "args":[["df", {"index_col": null}], ["pyeval", [["py", ["print(3.14+1); lasso"]]]]]}</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
   <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
xleash: AMIDST FIX element-dive loc-reporting.
[ci skip]
</commit_message>
<xml_diff>
--- a/tests/recursive.xlsx
+++ b/tests/recursive.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>#B1(D):..(DR):[“pipe”, [“odict”, “recurse”]]</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>#eval sheet!::{"opts": {"lax": true}, "func": "pipe", "args":[["df", {"index_col": null}], ["pyeval", [["py", ["print(3.14+1); lasso"]]]]]}</t>
+  </si>
+  <si>
+    <t>PevalAll</t>
+  </si>
+  <si>
+    <t>#eval sheet!::{"func": "pipe", "kwds":{"lax": false}, "args":[["df", {"index_col": null}], ["pyeval", {"include": "EVAL_COL", "eval_all": true}], "recurse"]}</t>
   </si>
 </sst>
 </file>
@@ -473,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -542,49 +548,57 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>31</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
xleash: AMIDST(2) FIX element-dive loc-reporting & df incl/excl.
+ tests: Improve stripped-str assertion.
[ci skip]
</commit_message>
<xml_diff>
--- a/tests/recursive.xlsx
+++ b/tests/recursive.xlsx
@@ -11,6 +11,7 @@
     <sheet name="3" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="3" r:id="rId3"/>
     <sheet name="eval sheet" sheetId="4" r:id="rId4"/>
+    <sheet name="e2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -124,10 +125,10 @@
     <t>#eval sheet!::{"opts": {"lax": true}, "func": "pipe", "args":[["df", {"index_col": null}], ["pyeval", [["py", ["print(3.14+1); lasso"]]]]]}</t>
   </si>
   <si>
-    <t>PevalAll</t>
-  </si>
-  <si>
     <t>#eval sheet!::{"func": "pipe", "kwds":{"lax": false}, "args":[["df", {"index_col": null}], ["pyeval", {"include": "EVAL_COL", "eval_all": true}], "recurse"]}</t>
+  </si>
+  <si>
+    <t>#B2</t>
   </si>
 </sst>
 </file>
@@ -482,7 +483,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -546,14 +547,6 @@
       </c>
       <c r="C9" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -788,6 +781,27 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
xleash: Simplify *filters arg for pyeval and recurse filters.
+ doc, sh-fact: Remove forgotten mention of "cur-sheet".
+ ALL TCs pass!
</commit_message>
<xml_diff>
--- a/tests/recursive.xlsx
+++ b/tests/recursive.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="1335" windowWidth="16380" windowHeight="8190" tabRatio="358"/>
+    <workbookView xWindow="2270" yWindow="1340" windowWidth="16380" windowHeight="8190" tabRatio="358"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="1" r:id="rId1"/>
@@ -122,13 +122,13 @@
     <t>bus</t>
   </si>
   <si>
-    <t>#eval sheet!::{"opts": {"lax": true}, "func": "pipe", "args":[["df", {"index_col": null}], ["pyeval", [["py", ["print(3.14+1); lasso"]]]]]}</t>
-  </si>
-  <si>
     <t>#eval sheet!::{"func": "pipe", "kwds":{"lax": false}, "args":[["df", {"index_col": null}], ["pyeval", {"include": "EVAL_COL", "eval_all": true}], "recurse"]}</t>
   </si>
   <si>
     <t>#B2</t>
+  </si>
+  <si>
+    <t>#eval sheet!::{"opts": {"lax": true}, "func": "pipe", "args":[["df", {"index_col": null}], ["pyeval", {"filters": [["py", ["print(3.14+1); lasso"]]]}]]}</t>
   </si>
 </sst>
 </file>
@@ -483,28 +483,28 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125"/>
-    <col min="2" max="2" width="31.140625"/>
-    <col min="3" max="3" width="37.42578125"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="27.54296875"/>
+    <col min="2" max="2" width="31.1796875"/>
+    <col min="3" max="3" width="37.453125"/>
+    <col min="4" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -512,7 +512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -520,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -528,7 +528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -536,25 +536,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>8</v>
       </c>
@@ -562,7 +562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -573,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -584,7 +584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -613,14 +613,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="20.85546875"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.54296875"/>
+    <col min="2" max="2" width="20.81640625"/>
+    <col min="3" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>11</v>
       </c>
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>21</v>
       </c>
@@ -648,7 +648,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5">
         <v>65</v>
@@ -657,16 +657,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -674,7 +674,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -682,7 +682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -701,22 +701,22 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col min="1" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F7">
         <v>3</v>
       </c>
@@ -739,9 +739,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -752,7 +752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
@@ -763,7 +763,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -774,7 +774,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>33</v>
       </c>
@@ -782,7 +782,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -796,11 +796,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>